<commit_message>
Changed hardlookup for Node ID, to look for any column with name equal to ID
</commit_message>
<xml_diff>
--- a/Objects.xlsx
+++ b/Objects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdfri\Documents\GitRepos\GraphViz_Tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdfri\Documents\GitRepos\githubExcelToGraph\ExcelToGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F54F01-0391-4086-B99E-3815AB4EB149}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E800AA-2856-4B3D-A7C3-E35D6FD1FBCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B60F0F70-B182-4D70-8FC1-7A5C0C86F9B0}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>IP</t>
   </si>
@@ -499,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485865F4-830E-43DB-AF9A-3777DC730EF0}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,41 +511,39 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -560,9 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE4DF79-7832-4901-BD35-0CFAF16A6B24}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -571,21 +564,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -597,9 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9102C3-7725-41FF-BADE-D66A4150419F}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -608,53 +599,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -677,18 +668,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -716,51 +707,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>